<commit_message>
fix: cambio estructura genItem.xlsx
</commit_message>
<xml_diff>
--- a/src/assets/ejemplos/modelo/GenItem.xlsx
+++ b/src/assets/ejemplos/modelo/GenItem.xlsx
@@ -204,16 +204,16 @@
     <t xml:space="preserve">Impuesto venta</t>
   </si>
   <si>
+    <t xml:space="preserve">Impuestoc compra</t>
+  </si>
+  <si>
     <t xml:space="preserve">Item prueba</t>
   </si>
   <si>
     <t xml:space="preserve">001</t>
   </si>
   <si>
-    <t xml:space="preserve">Prueba</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
+    <t xml:space="preserve">xyz</t>
   </si>
   <si>
     <t xml:space="preserve">Item prueba2</t>
@@ -222,7 +222,7 @@
     <t xml:space="preserve">002</t>
   </si>
   <si>
-    <t xml:space="preserve">PRUEBA2</t>
+    <t xml:space="preserve">abc</t>
   </si>
 </sst>
 </file>
@@ -325,7 +325,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -344,6 +344,10 @@
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -595,10 +599,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AK1048576"/>
+  <dimension ref="A1:AL1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="M3" activeCellId="0" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -614,6 +618,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="13.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="5.55"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="12.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="1" width="14.62"/>
   </cols>
   <sheetData>
     <row r="1" s="3" customFormat="true" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -656,7 +661,9 @@
       <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1"/>
+      <c r="N1" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
       <c r="Q1" s="1"/>
@@ -680,16 +687,17 @@
       <c r="AI1" s="1"/>
       <c r="AJ1" s="1"/>
       <c r="AK1" s="1"/>
+      <c r="AL1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D2" s="1" t="n">
         <v>10000</v>
@@ -703,14 +711,14 @@
       <c r="G2" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="H2" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="I2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J2" s="1" t="n">
-        <v>1</v>
+      <c r="H2" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="I2" s="5" t="n">
+        <v>110505</v>
+      </c>
+      <c r="J2" s="5" t="n">
+        <v>120599</v>
       </c>
       <c r="K2" s="1" t="n">
         <v>1</v>
@@ -722,7 +730,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="16.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>17</v>
       </c>
@@ -747,20 +755,20 @@
       <c r="H3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="I3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>1</v>
+      <c r="I3" s="5" t="n">
+        <v>110505</v>
+      </c>
+      <c r="J3" s="5" t="n">
+        <v>120599</v>
       </c>
       <c r="K3" s="1" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="L3" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="M3" s="1" t="n">
-        <v>2</v>
+        <v>0</v>
+      </c>
+      <c r="N3" s="1" t="n">
+        <v>3</v>
       </c>
     </row>
     <row r="1048568" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>

</xml_diff>